<commit_message>
ajustes no html e xlsx
</commit_message>
<xml_diff>
--- a/arquivos-planilhas/1.xlsx
+++ b/arquivos-planilhas/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Documents\GitHub\manipulacao_arquivos\arquivos-planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615EC2C7-A023-4087-8001-3D8FC9B4A749}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F0C9C4-9E85-4C4C-8F97-535B81BADFDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="127">
   <si>
     <t>Nome</t>
   </si>
@@ -447,11 +447,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +774,8 @@
   </sheetPr>
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1447,7 +1450,7 @@
       <c r="A65" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="4" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>